<commit_message>
docs: update parts list
</commit_message>
<xml_diff>
--- a/tutorial/parts-list.xlsx
+++ b/tutorial/parts-list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10119"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajayquirk/Library/CloudStorage/OneDrive-VictoriaUniversityofWellington-STUDENT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajayquirk/Documents/Restore Labs/grss-ir-nz/tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A944764-CAF5-5748-B216-2561E3B083FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C7C9838-AF6E-2347-B31C-65A09115D359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{95FDA46B-DB0F-8742-9189-533F54CD156F}"/>
+    <workbookView xWindow="1180" yWindow="880" windowWidth="34820" windowHeight="22500" xr2:uid="{95FDA46B-DB0F-8742-9189-533F54CD156F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -68,9 +68,6 @@
     <t>Ublox ANN-MB-02</t>
   </si>
   <si>
-    <t>https://www.digikey.co.nz/en/products/detail/u-blox/ANN-MB-02/9817927</t>
-  </si>
-  <si>
     <t>Header Kit for Feather - 12-pin and 16-pin Female Header Set</t>
   </si>
   <si>
@@ -198,6 +195,9 @@
   </si>
   <si>
     <t>Total Cost</t>
+  </si>
+  <si>
+    <t>https://www.digikey.co.nz/en/products/detail/u-blox/ANN-MB-00/9817928?s=N4IgTCBcDaIGwHYwFoCCA5dyCyAhZADAcugCIgC6AvkA</t>
   </si>
 </sst>
 </file>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338F21FE-813D-9941-9545-46CA0FDF8AE8}">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="187" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="187" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -692,7 +692,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="F2" s="8">
         <v>136.33250000000001</v>
@@ -700,19 +700,19 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="7">
         <v>1</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F3" s="8">
         <v>1.1499999999999999</v>
@@ -720,19 +720,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="8">
         <v>170.3</v>
@@ -740,19 +740,19 @@
     </row>
     <row r="5" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="7">
         <v>1</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="8">
         <v>209.9</v>
@@ -760,19 +760,19 @@
     </row>
     <row r="6" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>22</v>
       </c>
       <c r="D6" s="7">
         <v>1</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F6" s="8">
         <v>37.72</v>
@@ -780,19 +780,19 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="7">
         <v>2</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" s="8">
         <v>5.1289999999999996</v>
@@ -800,42 +800,42 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="7">
         <v>1</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F8" s="8">
         <v>23.9</v>
       </c>
       <c r="G8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="7">
         <v>1</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F9" s="8">
         <v>28.56</v>
@@ -843,19 +843,19 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D10" s="7">
         <v>1</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="8">
         <v>3.51</v>
@@ -863,287 +863,287 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="C15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="E32" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F32">
         <f>SUM(F2:F31)</f>

</xml_diff>